<commit_message>
Integrado ambiente de homologação
</commit_message>
<xml_diff>
--- a/excel/planilhasGerada/importar-parceiros.xlsx
+++ b/excel/planilhasGerada/importar-parceiros.xlsx
@@ -900,115 +900,51 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Cliente | Fornecedor</t>
+          <t>Fornecedor</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Pessoa Física</t>
+          <t>Estrangeiro</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>324.160.857-35</t>
+          <t>52160897302</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Emanuella Vieira</t>
+          <t>Igor Monteiro</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>09/12/1962</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="n">
-        <v>8332</v>
-      </c>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Contribuinte</t>
-        </is>
-      </c>
-      <c r="K3" t="n">
-        <v>2895</v>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>24794329</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Dr. João Lopes</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>519.462.380-15</t>
-        </is>
-      </c>
-      <c r="O3" s="6" t="inlineStr">
-        <is>
-          <t>orchestrate interactive eyeballs</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
+          <t>Isento</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" s="6" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
       <c r="S3" s="6" t="inlineStr"/>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>RESIDENCIAL</t>
-        </is>
-      </c>
-      <c r="U3" s="6" t="inlineStr">
-        <is>
-          <t>34481091</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>Rua Lucca Gonçalves</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>VCMC7YJ97A</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>Ouro Preto</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>Betânia</t>
-        </is>
-      </c>
-      <c r="AA3" s="6" t="inlineStr">
-        <is>
-          <t>GO</t>
-        </is>
-      </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>Brasil</t>
-        </is>
-      </c>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" s="6" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" s="6" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
     </row>
     <row r="4" ht="30" customHeight="1">
       <c r="A4" t="inlineStr">
@@ -1028,117 +964,41 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>348.056.217-53</t>
+          <t>253.169.870-12</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Dr. Yuri Sales</t>
+          <t>Maria Alice Peixoto</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>20/03/1978</t>
-        </is>
-      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="n">
-        <v>8462</v>
-      </c>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Contribuinte</t>
-        </is>
-      </c>
-      <c r="K4" t="n">
-        <v>3142</v>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>82252918</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Ana Vitória Fogaça</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>786.495.123-64</t>
-        </is>
-      </c>
-      <c r="O4" s="6" t="inlineStr">
-        <is>
-          <t>scale seamless deliverables</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>FAX</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>17893546093</t>
-        </is>
-      </c>
-      <c r="S4" s="6" t="inlineStr">
-        <is>
-          <t>julia71@hotmail.com</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>OUTROS</t>
-        </is>
-      </c>
-      <c r="U4" s="6" t="inlineStr">
-        <is>
-          <t>02903591</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>Avenida Ribeiro</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>76</t>
-        </is>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>YI7DRQJ33K</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>Dom Bosco</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>Trevo</t>
-        </is>
-      </c>
-      <c r="AA4" s="6" t="inlineStr">
-        <is>
-          <t>MA</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>Brasil</t>
-        </is>
-      </c>
+          <t>Isento</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" s="6" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" s="6" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" s="6" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" s="6" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
     </row>
     <row r="5" ht="30" customHeight="1">
       <c r="A5" t="inlineStr">
@@ -1148,127 +1008,53 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Cliente | Transportadora</t>
+          <t>Cliente | Fornecedor</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Pessoa Física</t>
+          <t>Estrangeiro</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>401.976.532-43</t>
+          <t>73215049805</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Enrico Melo</t>
+          <t>Natália Fogaça</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>04/04/1999</t>
-        </is>
-      </c>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="n">
-        <v>1804</v>
-      </c>
+      <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Não Contribuinte</t>
+          <t>Contribuinte</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>9489</v>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>24794329</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Pedro Mendes</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>492.615.037-99</t>
-        </is>
-      </c>
-      <c r="O5" s="6" t="inlineStr">
-        <is>
-          <t>empower collaborative interfaces</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>FAX</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>95742831005</t>
-        </is>
-      </c>
-      <c r="S5" s="6" t="inlineStr">
-        <is>
-          <t>martinsyago@uol.com.br</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>ENTREGA</t>
-        </is>
-      </c>
-      <c r="U5" s="6" t="inlineStr">
-        <is>
-          <t>05546152</t>
-        </is>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>Vale Pires</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>84</t>
-        </is>
-      </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>P8G6K5TBMA</t>
-        </is>
-      </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>Nossa Senhora De Fátima</t>
-        </is>
-      </c>
-      <c r="Z5" t="inlineStr">
-        <is>
-          <t>Vera Cruz</t>
-        </is>
-      </c>
-      <c r="AA5" s="6" t="inlineStr">
-        <is>
-          <t>SP</t>
-        </is>
-      </c>
-      <c r="AB5" t="inlineStr">
-        <is>
-          <t>Brasil</t>
-        </is>
-      </c>
+        <v>6967</v>
+      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" s="6" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" s="6" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" s="6" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" s="6" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
     </row>
     <row r="6" ht="30" customHeight="1">
       <c r="A6" t="inlineStr">
@@ -1278,34 +1064,28 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Transportadora</t>
+          <t>Cliente | Transportadora</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Pessoa Física</t>
+          <t>Estrangeiro</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>625.843.790-74</t>
+          <t>87254619076</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Enrico Rocha</t>
+          <t>Eduarda Ribeiro</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>06/08/1969</t>
-        </is>
-      </c>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
-      <c r="I6" t="n">
-        <v>8164</v>
-      </c>
+      <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr">
         <is>
           <t>Isento</t>
@@ -1313,74 +1093,22 @@
       </c>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>Srta. Letícia Santos</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>150.293.867-77</t>
-        </is>
-      </c>
-      <c r="O6" s="6" t="inlineStr">
-        <is>
-          <t>e-enable visionary web-readiness</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" s="6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr"/>
       <c r="S6" s="6" t="inlineStr"/>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>COBRANCA</t>
-        </is>
-      </c>
-      <c r="U6" s="6" t="inlineStr">
-        <is>
-          <t>80823427</t>
-        </is>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>Campo da Cruz</t>
-        </is>
-      </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>KJOWBK084M</t>
-        </is>
-      </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>Maravilha</t>
-        </is>
-      </c>
-      <c r="Z6" t="inlineStr">
-        <is>
-          <t>Barroca</t>
-        </is>
-      </c>
-      <c r="AA6" s="6" t="inlineStr">
-        <is>
-          <t>AL</t>
-        </is>
-      </c>
-      <c r="AB6" t="inlineStr">
-        <is>
-          <t>Brasil</t>
-        </is>
-      </c>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" s="6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" s="6" t="inlineStr"/>
+      <c r="AB6" t="inlineStr"/>
     </row>
     <row r="7" ht="30" customHeight="1">
       <c r="A7" t="inlineStr">
@@ -1390,38 +1118,28 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Cliente | Transportadora</t>
+          <t>Transportadora</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Pessoa Jurídica</t>
+          <t>Pessoa Física</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>60.538.129/0001-80</t>
+          <t>870.249.615-11</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>João Gabriel Nascimento</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>iterate turn-key platforms</t>
-        </is>
-      </c>
+          <t>Joana Rodrigues</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>3250706</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
-        <v>1541</v>
-      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
           <t>Isento</t>
@@ -1429,74 +1147,22 @@
       </c>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>Thomas Santos</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>51.462.370/0001-81</t>
-        </is>
-      </c>
-      <c r="O7" s="6" t="inlineStr">
-        <is>
-          <t>strategize seamless vortals</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" s="6" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr"/>
       <c r="S7" s="6" t="inlineStr"/>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>OUTROS</t>
-        </is>
-      </c>
-      <c r="U7" s="6" t="inlineStr">
-        <is>
-          <t>23853792</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>Vila da Luz</t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>37</t>
-        </is>
-      </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>0N7CKVZU1G</t>
-        </is>
-      </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>Boa Esperança</t>
-        </is>
-      </c>
-      <c r="Z7" t="inlineStr">
-        <is>
-          <t>Vila Da Amizade</t>
-        </is>
-      </c>
-      <c r="AA7" s="6" t="inlineStr">
-        <is>
-          <t>MA</t>
-        </is>
-      </c>
-      <c r="AB7" t="inlineStr">
-        <is>
-          <t>Brasil</t>
-        </is>
-      </c>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" s="6" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
+      <c r="Z7" t="inlineStr"/>
+      <c r="AA7" s="6" t="inlineStr"/>
+      <c r="AB7" t="inlineStr"/>
     </row>
     <row r="8" ht="30" customHeight="1">
       <c r="A8" t="inlineStr">
@@ -1506,131 +1172,53 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Fornecedor | Transportadora</t>
+          <t>Cliente</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Pessoa Jurídica</t>
+          <t>Estrangeiro</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>31.802.547/0001-34</t>
+          <t>47836012913</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Ana Lívia Pereira</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>empower clicks-and-mortar e-commerce</t>
-        </is>
-      </c>
+          <t>Luiz Otávio Moreira</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>3250706</t>
-        </is>
-      </c>
-      <c r="I8" t="n">
-        <v>8538</v>
-      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Contribuinte</t>
+          <t>Não Contribuinte</t>
         </is>
       </c>
       <c r="K8" t="n">
-        <v>349</v>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>82252918</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>Heloísa Gomes</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>19.240.635/0001-94</t>
-        </is>
-      </c>
-      <c r="O8" s="6" t="inlineStr">
-        <is>
-          <t>integrate bricks-and-clicks paradigms</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>FAX</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>27958604300</t>
-        </is>
-      </c>
-      <c r="S8" s="6" t="inlineStr">
-        <is>
-          <t>rodriguesthales@hotmail.com</t>
-        </is>
-      </c>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>RESIDENCIAL</t>
-        </is>
-      </c>
-      <c r="U8" s="6" t="inlineStr">
-        <is>
-          <t>40134292</t>
-        </is>
-      </c>
-      <c r="V8" t="inlineStr">
-        <is>
-          <t>Feira Correia</t>
-        </is>
-      </c>
-      <c r="W8" t="inlineStr">
-        <is>
-          <t>83</t>
-        </is>
-      </c>
-      <c r="X8" t="inlineStr">
-        <is>
-          <t>IAH17ZQ92Y</t>
-        </is>
-      </c>
-      <c r="Y8" t="inlineStr">
-        <is>
-          <t>Vila São Gabriel</t>
-        </is>
-      </c>
-      <c r="Z8" t="inlineStr">
-        <is>
-          <t>Europa</t>
-        </is>
-      </c>
-      <c r="AA8" s="6" t="inlineStr">
-        <is>
-          <t>GO</t>
-        </is>
-      </c>
-      <c r="AB8" t="inlineStr">
-        <is>
-          <t>Brasil</t>
-        </is>
-      </c>
+        <v>5657</v>
+      </c>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" s="6" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" s="6" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" s="6" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
+      <c r="Z8" t="inlineStr"/>
+      <c r="AA8" s="6" t="inlineStr"/>
+      <c r="AB8" t="inlineStr"/>
     </row>
     <row r="9" ht="30" customHeight="1">
       <c r="A9" t="inlineStr">
@@ -1640,115 +1228,51 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Cliente</t>
+          <t>Transportadora</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Pessoa Física</t>
+          <t>Pessoa Jurídica</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>105.246.783-08</t>
+          <t>86.401.275/0001-52</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Diogo Vieira</t>
+          <t>Caroline da Mata</t>
         </is>
       </c>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>15/07/1990</t>
-        </is>
-      </c>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
-      <c r="I9" t="n">
-        <v>963</v>
-      </c>
+      <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Contribuinte</t>
-        </is>
-      </c>
-      <c r="K9" t="n">
-        <v>323</v>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>24794329</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>Igor Silva</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>498.507.613-93</t>
-        </is>
-      </c>
-      <c r="O9" s="6" t="inlineStr">
-        <is>
-          <t>orchestrate vertical e-commerce</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
+          <t>Isento</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" s="6" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr"/>
       <c r="S9" s="6" t="inlineStr"/>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>COMERCIAL</t>
-        </is>
-      </c>
-      <c r="U9" s="6" t="inlineStr">
-        <is>
-          <t>84737868</t>
-        </is>
-      </c>
-      <c r="V9" t="inlineStr">
-        <is>
-          <t>Chácara Gonçalves</t>
-        </is>
-      </c>
-      <c r="W9" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
-      </c>
-      <c r="X9" t="inlineStr">
-        <is>
-          <t>URKZQAUBH6</t>
-        </is>
-      </c>
-      <c r="Y9" t="inlineStr">
-        <is>
-          <t>Custodinha</t>
-        </is>
-      </c>
-      <c r="Z9" t="inlineStr">
-        <is>
-          <t>Monsenhor Messias</t>
-        </is>
-      </c>
-      <c r="AA9" s="6" t="inlineStr">
-        <is>
-          <t>GO</t>
-        </is>
-      </c>
-      <c r="AB9" t="inlineStr">
-        <is>
-          <t>Brasil</t>
-        </is>
-      </c>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" s="6" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr"/>
+      <c r="AA9" s="6" t="inlineStr"/>
+      <c r="AB9" t="inlineStr"/>
     </row>
     <row r="10" ht="30" customHeight="1">
       <c r="A10" t="inlineStr">
@@ -1758,7 +1282,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Cliente | Transportadora</t>
+          <t>Transportadora</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1768,109 +1292,43 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>27.386.054/0001-93</t>
+          <t>21.069.735/0001-41</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Enzo Fernandes</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>cultivate value-added supply-chains</t>
-        </is>
-      </c>
+          <t>Maria Pereira</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>4613300</t>
-        </is>
-      </c>
-      <c r="I10" t="n">
-        <v>8510</v>
-      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Não Contribuinte</t>
+          <t>Contribuinte</t>
         </is>
       </c>
       <c r="K10" t="n">
-        <v>4246</v>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>24794329</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>Maria Luiza Duarte</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>38.902.145/0001-50</t>
-        </is>
-      </c>
-      <c r="O10" s="6" t="inlineStr">
-        <is>
-          <t>iterate user-centric functionalities</t>
-        </is>
-      </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
+        <v>2823</v>
+      </c>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" s="6" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="inlineStr"/>
       <c r="S10" s="6" t="inlineStr"/>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>OUTROS</t>
-        </is>
-      </c>
-      <c r="U10" s="6" t="inlineStr">
-        <is>
-          <t>41173128</t>
-        </is>
-      </c>
-      <c r="V10" t="inlineStr">
-        <is>
-          <t>Viaduto Cunha</t>
-        </is>
-      </c>
-      <c r="W10" t="inlineStr">
-        <is>
-          <t>71</t>
-        </is>
-      </c>
-      <c r="X10" t="inlineStr">
-        <is>
-          <t>V4WADTRVQP</t>
-        </is>
-      </c>
-      <c r="Y10" t="inlineStr">
-        <is>
-          <t>Alto Vera Cruz</t>
-        </is>
-      </c>
-      <c r="Z10" t="inlineStr">
-        <is>
-          <t>Vila Suzana Segunda Seção</t>
-        </is>
-      </c>
-      <c r="AA10" s="6" t="inlineStr">
-        <is>
-          <t>SP</t>
-        </is>
-      </c>
-      <c r="AB10" t="inlineStr">
-        <is>
-          <t>Brasil</t>
-        </is>
-      </c>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" s="6" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr"/>
+      <c r="AA10" s="6" t="inlineStr"/>
+      <c r="AB10" t="inlineStr"/>
     </row>
     <row r="11" ht="30" customHeight="1">
       <c r="A11" t="inlineStr">
@@ -1885,106 +1343,48 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Estrangeiro</t>
+          <t>Pessoa Jurídica</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>46981072530</t>
+          <t>93.416.502/0001-89</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Diego Ferreira</t>
+          <t>Isabella da Rocha</t>
         </is>
       </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
-      <c r="I11" t="n">
-        <v>7470</v>
-      </c>
+      <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Não Contribuinte</t>
+          <t>Contribuinte</t>
         </is>
       </c>
       <c r="K11" t="n">
-        <v>592</v>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>87866990</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>Yuri Ferreira</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>53240816989</t>
-        </is>
-      </c>
-      <c r="O11" s="6" t="inlineStr">
-        <is>
-          <t>matrix vertical eyeballs</t>
-        </is>
-      </c>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
+        <v>8886</v>
+      </c>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" s="6" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="inlineStr"/>
       <c r="S11" s="6" t="inlineStr"/>
-      <c r="T11" t="inlineStr">
-        <is>
-          <t>COMERCIAL</t>
-        </is>
-      </c>
-      <c r="U11" s="6" t="inlineStr">
-        <is>
-          <t>52528193</t>
-        </is>
-      </c>
-      <c r="V11" t="inlineStr">
-        <is>
-          <t>Viela Ribeiro</t>
-        </is>
-      </c>
-      <c r="W11" t="inlineStr">
-        <is>
-          <t>86</t>
-        </is>
-      </c>
-      <c r="X11" t="inlineStr">
-        <is>
-          <t>3DFJO6UTNB</t>
-        </is>
-      </c>
-      <c r="Y11" t="inlineStr">
-        <is>
-          <t>Tiradentes</t>
-        </is>
-      </c>
-      <c r="Z11" t="inlineStr">
-        <is>
-          <t>Sagrada Família</t>
-        </is>
-      </c>
-      <c r="AA11" s="6" t="inlineStr">
-        <is>
-          <t>BA</t>
-        </is>
-      </c>
-      <c r="AB11" t="inlineStr">
-        <is>
-          <t>Brasil</t>
-        </is>
-      </c>
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" s="6" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
+      <c r="X11" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
+      <c r="Z11" t="inlineStr"/>
+      <c r="AA11" s="6" t="inlineStr"/>
+      <c r="AB11" t="inlineStr"/>
     </row>
     <row r="12" ht="30" customHeight="1">
       <c r="A12" t="inlineStr">
@@ -1994,127 +1394,53 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Fornecedor</t>
+          <t>Cliente | Fornecedor</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Pessoa Física</t>
+          <t>Estrangeiro</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>523.164.798-55</t>
+          <t>75638042938</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Maysa Silveira</t>
+          <t>Vinicius da Mata</t>
         </is>
       </c>
       <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>31/03/1971</t>
-        </is>
-      </c>
+      <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
-      <c r="I12" t="n">
-        <v>977</v>
-      </c>
+      <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Não Contribuinte</t>
+          <t>Contribuinte</t>
         </is>
       </c>
       <c r="K12" t="n">
-        <v>2288</v>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>87866990</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>Benício Silva</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>961.204.753-70</t>
-        </is>
-      </c>
-      <c r="O12" s="6" t="inlineStr">
-        <is>
-          <t>e-enable rich bandwidth</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>FAX</t>
-        </is>
-      </c>
-      <c r="R12" t="inlineStr">
-        <is>
-          <t>28694370565</t>
-        </is>
-      </c>
-      <c r="S12" s="6" t="inlineStr">
-        <is>
-          <t>bruno38@hotmail.com</t>
-        </is>
-      </c>
-      <c r="T12" t="inlineStr">
-        <is>
-          <t>OUTROS</t>
-        </is>
-      </c>
-      <c r="U12" s="6" t="inlineStr">
-        <is>
-          <t>84544886</t>
-        </is>
-      </c>
-      <c r="V12" t="inlineStr">
-        <is>
-          <t>Fazenda de Almeida</t>
-        </is>
-      </c>
-      <c r="W12" t="inlineStr">
-        <is>
-          <t>75</t>
-        </is>
-      </c>
-      <c r="X12" t="inlineStr">
-        <is>
-          <t>XM2SIKQRZE</t>
-        </is>
-      </c>
-      <c r="Y12" t="inlineStr">
-        <is>
-          <t>Vila Dos Anjos</t>
-        </is>
-      </c>
-      <c r="Z12" t="inlineStr">
-        <is>
-          <t>Conjunto Serra Verde</t>
-        </is>
-      </c>
-      <c r="AA12" s="6" t="inlineStr">
-        <is>
-          <t>SE</t>
-        </is>
-      </c>
-      <c r="AB12" t="inlineStr">
-        <is>
-          <t>Brasil</t>
-        </is>
-      </c>
+        <v>9603</v>
+      </c>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" s="6" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" s="6" t="inlineStr"/>
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" s="6" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
+      <c r="X12" t="inlineStr"/>
+      <c r="Y12" t="inlineStr"/>
+      <c r="Z12" t="inlineStr"/>
+      <c r="AA12" s="6" t="inlineStr"/>
+      <c r="AB12" t="inlineStr"/>
     </row>
     <row r="13" ht="30" customHeight="1">
       <c r="A13" t="inlineStr">
@@ -2124,263 +1450,1271 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>Fornecedor | Transportadora</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Pessoa Jurídica</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>51.809.347/0001-10</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Otávio Barbosa</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Isento</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" s="6" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" s="6" t="inlineStr"/>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" s="6" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
+      <c r="X13" t="inlineStr"/>
+      <c r="Y13" t="inlineStr"/>
+      <c r="Z13" t="inlineStr"/>
+      <c r="AA13" s="6" t="inlineStr"/>
+      <c r="AB13" t="inlineStr"/>
+    </row>
+    <row r="14" ht="30" customHeight="1">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Fornecedor | Transportadora</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Estrangeiro</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>06974381557</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Diego Gonçalves</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Isento</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" s="6" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" s="6" t="inlineStr"/>
+      <c r="T14" t="inlineStr"/>
+      <c r="U14" s="6" t="inlineStr"/>
+      <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
+      <c r="X14" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
+      <c r="Z14" t="inlineStr"/>
+      <c r="AA14" s="6" t="inlineStr"/>
+      <c r="AB14" t="inlineStr"/>
+    </row>
+    <row r="15" ht="30" customHeight="1">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Transportadora</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Estrangeiro</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>83607941203</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Maria Eduarda da Luz</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Contribuinte</t>
+        </is>
+      </c>
+      <c r="K15" t="n">
+        <v>3945</v>
+      </c>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" s="6" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr"/>
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" s="6" t="inlineStr"/>
+      <c r="T15" t="inlineStr"/>
+      <c r="U15" s="6" t="inlineStr"/>
+      <c r="V15" t="inlineStr"/>
+      <c r="W15" t="inlineStr"/>
+      <c r="X15" t="inlineStr"/>
+      <c r="Y15" t="inlineStr"/>
+      <c r="Z15" t="inlineStr"/>
+      <c r="AA15" s="6" t="inlineStr"/>
+      <c r="AB15" t="inlineStr"/>
+    </row>
+    <row r="16" ht="30" customHeight="1">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>Cliente | Fornecedor</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Pessoa Física</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>290.438.671-87</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>André Aragão</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Contribuinte</t>
+        </is>
+      </c>
+      <c r="K16" t="n">
+        <v>7108</v>
+      </c>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" s="6" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" s="6" t="inlineStr"/>
+      <c r="T16" t="inlineStr"/>
+      <c r="U16" s="6" t="inlineStr"/>
+      <c r="V16" t="inlineStr"/>
+      <c r="W16" t="inlineStr"/>
+      <c r="X16" t="inlineStr"/>
+      <c r="Y16" t="inlineStr"/>
+      <c r="Z16" t="inlineStr"/>
+      <c r="AA16" s="6" t="inlineStr"/>
+      <c r="AB16" t="inlineStr"/>
+    </row>
+    <row r="17" ht="30" customHeight="1">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Fornecedor</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Estrangeiro</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>05426897310</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Manuela Duarte</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Contribuinte</t>
+        </is>
+      </c>
+      <c r="K17" t="n">
+        <v>6968</v>
+      </c>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" s="6" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" s="6" t="inlineStr"/>
+      <c r="T17" t="inlineStr"/>
+      <c r="U17" s="6" t="inlineStr"/>
+      <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
+      <c r="X17" t="inlineStr"/>
+      <c r="Y17" t="inlineStr"/>
+      <c r="Z17" t="inlineStr"/>
+      <c r="AA17" s="6" t="inlineStr"/>
+      <c r="AB17" t="inlineStr"/>
+    </row>
+    <row r="18" ht="30" customHeight="1">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Cliente | Fornecedor | Transportadora</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Estrangeiro</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>29760581302</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Dra. Alana Gonçalves</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Não Contribuinte</t>
+        </is>
+      </c>
+      <c r="K18" t="n">
+        <v>1271</v>
+      </c>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" s="6" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" s="6" t="inlineStr"/>
+      <c r="T18" t="inlineStr"/>
+      <c r="U18" s="6" t="inlineStr"/>
+      <c r="V18" t="inlineStr"/>
+      <c r="W18" t="inlineStr"/>
+      <c r="X18" t="inlineStr"/>
+      <c r="Y18" t="inlineStr"/>
+      <c r="Z18" t="inlineStr"/>
+      <c r="AA18" s="6" t="inlineStr"/>
+      <c r="AB18" t="inlineStr"/>
+    </row>
+    <row r="19" ht="30" customHeight="1">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Fornecedor</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Pessoa Física</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>326.481.597-46</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Isis Duarte</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Não Contribuinte</t>
+        </is>
+      </c>
+      <c r="K19" t="n">
+        <v>4828</v>
+      </c>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" s="6" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" s="6" t="inlineStr"/>
+      <c r="T19" t="inlineStr"/>
+      <c r="U19" s="6" t="inlineStr"/>
+      <c r="V19" t="inlineStr"/>
+      <c r="W19" t="inlineStr"/>
+      <c r="X19" t="inlineStr"/>
+      <c r="Y19" t="inlineStr"/>
+      <c r="Z19" t="inlineStr"/>
+      <c r="AA19" s="6" t="inlineStr"/>
+      <c r="AB19" t="inlineStr"/>
+    </row>
+    <row r="20" ht="30" customHeight="1">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Fornecedor</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
         <is>
           <t>Pessoa Jurídica</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>81.769.324/0001-90</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Renan Barros</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>brand enterprise convergence</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>4613300</t>
-        </is>
-      </c>
-      <c r="I13" t="n">
-        <v>9791</v>
-      </c>
-      <c r="J13" t="inlineStr">
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>81.479.653/0001-05</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Diego Freitas</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Isento</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" s="6" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" s="6" t="inlineStr"/>
+      <c r="T20" t="inlineStr"/>
+      <c r="U20" s="6" t="inlineStr"/>
+      <c r="V20" t="inlineStr"/>
+      <c r="W20" t="inlineStr"/>
+      <c r="X20" t="inlineStr"/>
+      <c r="Y20" t="inlineStr"/>
+      <c r="Z20" t="inlineStr"/>
+      <c r="AA20" s="6" t="inlineStr"/>
+      <c r="AB20" t="inlineStr"/>
+    </row>
+    <row r="21" ht="30" customHeight="1">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Fornecedor</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Estrangeiro</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>72350918432</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>João Miguel da Costa</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Não Contribuinte</t>
+        </is>
+      </c>
+      <c r="K21" t="n">
+        <v>3190</v>
+      </c>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" s="6" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" s="6" t="inlineStr"/>
+      <c r="T21" t="inlineStr"/>
+      <c r="U21" s="6" t="inlineStr"/>
+      <c r="V21" t="inlineStr"/>
+      <c r="W21" t="inlineStr"/>
+      <c r="X21" t="inlineStr"/>
+      <c r="Y21" t="inlineStr"/>
+      <c r="Z21" t="inlineStr"/>
+      <c r="AA21" s="6" t="inlineStr"/>
+      <c r="AB21" t="inlineStr"/>
+    </row>
+    <row r="22" ht="30" customHeight="1">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Fornecedor</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Pessoa Física</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>314.985.076-20</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Pedro Henrique Almeida</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Isento</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" s="6" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" s="6" t="inlineStr"/>
+      <c r="T22" t="inlineStr"/>
+      <c r="U22" s="6" t="inlineStr"/>
+      <c r="V22" t="inlineStr"/>
+      <c r="W22" t="inlineStr"/>
+      <c r="X22" t="inlineStr"/>
+      <c r="Y22" t="inlineStr"/>
+      <c r="Z22" t="inlineStr"/>
+      <c r="AA22" s="6" t="inlineStr"/>
+      <c r="AB22" t="inlineStr"/>
+    </row>
+    <row r="23" ht="30" customHeight="1">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Cliente | Transportadora</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Estrangeiro</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>83752910640</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Kaique Moura</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Isento</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" s="6" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" s="6" t="inlineStr"/>
+      <c r="T23" t="inlineStr"/>
+      <c r="U23" s="6" t="inlineStr"/>
+      <c r="V23" t="inlineStr"/>
+      <c r="W23" t="inlineStr"/>
+      <c r="X23" t="inlineStr"/>
+      <c r="Y23" t="inlineStr"/>
+      <c r="Z23" t="inlineStr"/>
+      <c r="AA23" s="6" t="inlineStr"/>
+      <c r="AB23" t="inlineStr"/>
+    </row>
+    <row r="24" ht="30" customHeight="1">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Cliente | Fornecedor</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Estrangeiro</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>23564879056</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Ana Sophia Campos</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr">
         <is>
           <t>Contribuinte</t>
         </is>
       </c>
-      <c r="K13" t="n">
-        <v>2974</v>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>87866990</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>Rafaela da Cunha</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>31.827.095/0001-45</t>
-        </is>
-      </c>
-      <c r="O13" s="6" t="inlineStr">
-        <is>
-          <t>visualize cutting-edge methodologies</t>
-        </is>
-      </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>Residencial</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>67809532103</t>
-        </is>
-      </c>
-      <c r="S13" s="6" t="inlineStr">
-        <is>
-          <t>calebe85@gmail.com</t>
-        </is>
-      </c>
-      <c r="T13" t="inlineStr">
-        <is>
-          <t>ENTREGA</t>
-        </is>
-      </c>
-      <c r="U13" s="6" t="inlineStr">
-        <is>
-          <t>60322651</t>
-        </is>
-      </c>
-      <c r="V13" t="inlineStr">
-        <is>
-          <t>Setor Silveira</t>
-        </is>
-      </c>
-      <c r="W13" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
-      <c r="X13" t="inlineStr">
-        <is>
-          <t>UZ0UU64P7J</t>
-        </is>
-      </c>
-      <c r="Y13" t="inlineStr">
-        <is>
-          <t>Mariquinhas</t>
-        </is>
-      </c>
-      <c r="Z13" t="inlineStr">
-        <is>
-          <t>Vila Cemig</t>
-        </is>
-      </c>
-      <c r="AA13" s="6" t="inlineStr">
-        <is>
-          <t>RO</t>
-        </is>
-      </c>
-      <c r="AB13" t="inlineStr">
-        <is>
-          <t>Brasil</t>
-        </is>
-      </c>
-    </row>
-    <row r="14" ht="30" customHeight="1">
-      <c r="O14" s="6" t="n"/>
-      <c r="S14" s="6" t="n"/>
-      <c r="U14" s="6" t="n"/>
-      <c r="AA14" s="6" t="n"/>
-    </row>
-    <row r="15" ht="30" customHeight="1">
-      <c r="O15" s="6" t="n"/>
-      <c r="S15" s="6" t="n"/>
-      <c r="U15" s="6" t="n"/>
-      <c r="AA15" s="6" t="n"/>
-    </row>
-    <row r="16" ht="30" customHeight="1">
-      <c r="O16" s="6" t="n"/>
-      <c r="S16" s="6" t="n"/>
-      <c r="U16" s="6" t="n"/>
-      <c r="AA16" s="6" t="n"/>
-    </row>
-    <row r="17" ht="30" customHeight="1">
-      <c r="O17" s="6" t="n"/>
-      <c r="S17" s="6" t="n"/>
-      <c r="U17" s="6" t="n"/>
-      <c r="AA17" s="6" t="n"/>
-    </row>
-    <row r="18" ht="30" customHeight="1">
-      <c r="O18" s="6" t="n"/>
-      <c r="S18" s="6" t="n"/>
-      <c r="U18" s="6" t="n"/>
-      <c r="AA18" s="6" t="n"/>
-    </row>
-    <row r="19" ht="30" customHeight="1">
-      <c r="O19" s="6" t="n"/>
-      <c r="S19" s="6" t="n"/>
-      <c r="U19" s="6" t="n"/>
-      <c r="AA19" s="6" t="n"/>
-    </row>
-    <row r="20" ht="30" customHeight="1">
-      <c r="O20" s="6" t="n"/>
-      <c r="S20" s="6" t="n"/>
-      <c r="U20" s="6" t="n"/>
-      <c r="AA20" s="6" t="n"/>
-    </row>
-    <row r="21" ht="30" customHeight="1">
-      <c r="O21" s="6" t="n"/>
-      <c r="S21" s="6" t="n"/>
-      <c r="U21" s="6" t="n"/>
-      <c r="AA21" s="6" t="n"/>
-    </row>
-    <row r="22" ht="30" customHeight="1">
-      <c r="O22" s="6" t="n"/>
-      <c r="S22" s="6" t="n"/>
-      <c r="U22" s="6" t="n"/>
-      <c r="AA22" s="6" t="n"/>
-    </row>
-    <row r="23" ht="30" customHeight="1">
-      <c r="O23" s="6" t="n"/>
-      <c r="S23" s="6" t="n"/>
-      <c r="U23" s="6" t="n"/>
-      <c r="AA23" s="6" t="n"/>
-    </row>
-    <row r="24" ht="30" customHeight="1">
-      <c r="O24" s="6" t="n"/>
-      <c r="S24" s="6" t="n"/>
-      <c r="U24" s="6" t="n"/>
-      <c r="AA24" s="6" t="n"/>
+      <c r="K24" t="n">
+        <v>8775</v>
+      </c>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" s="6" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr"/>
+      <c r="R24" t="inlineStr"/>
+      <c r="S24" s="6" t="inlineStr"/>
+      <c r="T24" t="inlineStr"/>
+      <c r="U24" s="6" t="inlineStr"/>
+      <c r="V24" t="inlineStr"/>
+      <c r="W24" t="inlineStr"/>
+      <c r="X24" t="inlineStr"/>
+      <c r="Y24" t="inlineStr"/>
+      <c r="Z24" t="inlineStr"/>
+      <c r="AA24" s="6" t="inlineStr"/>
+      <c r="AB24" t="inlineStr"/>
     </row>
     <row r="25" ht="30" customHeight="1">
-      <c r="O25" s="6" t="n"/>
-      <c r="S25" s="6" t="n"/>
-      <c r="U25" s="6" t="n"/>
-      <c r="AA25" s="6" t="n"/>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Cliente</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Pessoa Física</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>253.098.761-03</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Erick da Cunha</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Contribuinte</t>
+        </is>
+      </c>
+      <c r="K25" t="n">
+        <v>122</v>
+      </c>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" s="6" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="inlineStr"/>
+      <c r="R25" t="inlineStr"/>
+      <c r="S25" s="6" t="inlineStr"/>
+      <c r="T25" t="inlineStr"/>
+      <c r="U25" s="6" t="inlineStr"/>
+      <c r="V25" t="inlineStr"/>
+      <c r="W25" t="inlineStr"/>
+      <c r="X25" t="inlineStr"/>
+      <c r="Y25" t="inlineStr"/>
+      <c r="Z25" t="inlineStr"/>
+      <c r="AA25" s="6" t="inlineStr"/>
+      <c r="AB25" t="inlineStr"/>
     </row>
     <row r="26" ht="30" customHeight="1">
-      <c r="O26" s="6" t="n"/>
-      <c r="S26" s="6" t="n"/>
-      <c r="U26" s="6" t="n"/>
-      <c r="AA26" s="6" t="n"/>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Cliente</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Estrangeiro</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>07346982169</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Ana Laura da Mata</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Não Contribuinte</t>
+        </is>
+      </c>
+      <c r="K26" t="n">
+        <v>1584</v>
+      </c>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
+      <c r="O26" s="6" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="inlineStr"/>
+      <c r="R26" t="inlineStr"/>
+      <c r="S26" s="6" t="inlineStr"/>
+      <c r="T26" t="inlineStr"/>
+      <c r="U26" s="6" t="inlineStr"/>
+      <c r="V26" t="inlineStr"/>
+      <c r="W26" t="inlineStr"/>
+      <c r="X26" t="inlineStr"/>
+      <c r="Y26" t="inlineStr"/>
+      <c r="Z26" t="inlineStr"/>
+      <c r="AA26" s="6" t="inlineStr"/>
+      <c r="AB26" t="inlineStr"/>
     </row>
     <row r="27" ht="30" customHeight="1">
-      <c r="O27" s="6" t="n"/>
-      <c r="S27" s="6" t="n"/>
-      <c r="U27" s="6" t="n"/>
-      <c r="AA27" s="6" t="n"/>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Transportadora</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Pessoa Física</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>784.206.593-47</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Yago Novaes</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Contribuinte</t>
+        </is>
+      </c>
+      <c r="K27" t="n">
+        <v>5320</v>
+      </c>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" s="6" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr"/>
+      <c r="R27" t="inlineStr"/>
+      <c r="S27" s="6" t="inlineStr"/>
+      <c r="T27" t="inlineStr"/>
+      <c r="U27" s="6" t="inlineStr"/>
+      <c r="V27" t="inlineStr"/>
+      <c r="W27" t="inlineStr"/>
+      <c r="X27" t="inlineStr"/>
+      <c r="Y27" t="inlineStr"/>
+      <c r="Z27" t="inlineStr"/>
+      <c r="AA27" s="6" t="inlineStr"/>
+      <c r="AB27" t="inlineStr"/>
     </row>
     <row r="28" ht="30" customHeight="1">
-      <c r="O28" s="6" t="n"/>
-      <c r="S28" s="6" t="n"/>
-      <c r="U28" s="6" t="n"/>
-      <c r="AA28" s="6" t="n"/>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Cliente | Transportadora</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Pessoa Jurídica</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>05.639.287/0001-18</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Emilly Melo</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Contribuinte</t>
+        </is>
+      </c>
+      <c r="K28" t="n">
+        <v>1924</v>
+      </c>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" s="6" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr"/>
+      <c r="R28" t="inlineStr"/>
+      <c r="S28" s="6" t="inlineStr"/>
+      <c r="T28" t="inlineStr"/>
+      <c r="U28" s="6" t="inlineStr"/>
+      <c r="V28" t="inlineStr"/>
+      <c r="W28" t="inlineStr"/>
+      <c r="X28" t="inlineStr"/>
+      <c r="Y28" t="inlineStr"/>
+      <c r="Z28" t="inlineStr"/>
+      <c r="AA28" s="6" t="inlineStr"/>
+      <c r="AB28" t="inlineStr"/>
     </row>
     <row r="29" ht="30" customHeight="1">
-      <c r="O29" s="6" t="n"/>
-      <c r="S29" s="6" t="n"/>
-      <c r="U29" s="6" t="n"/>
-      <c r="AA29" s="6" t="n"/>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Cliente</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Pessoa Jurídica</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>10.692.738/0001-10</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Sr. Fernando da Conceição</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Isento</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr"/>
+      <c r="O29" s="6" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr"/>
+      <c r="R29" t="inlineStr"/>
+      <c r="S29" s="6" t="inlineStr"/>
+      <c r="T29" t="inlineStr"/>
+      <c r="U29" s="6" t="inlineStr"/>
+      <c r="V29" t="inlineStr"/>
+      <c r="W29" t="inlineStr"/>
+      <c r="X29" t="inlineStr"/>
+      <c r="Y29" t="inlineStr"/>
+      <c r="Z29" t="inlineStr"/>
+      <c r="AA29" s="6" t="inlineStr"/>
+      <c r="AB29" t="inlineStr"/>
     </row>
     <row r="30" ht="30" customHeight="1">
-      <c r="O30" s="6" t="n"/>
-      <c r="S30" s="6" t="n"/>
-      <c r="U30" s="6" t="n"/>
-      <c r="AA30" s="6" t="n"/>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Cliente | Transportadora</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Pessoa Física</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>874.051.936-84</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Olivia da Rocha</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Contribuinte</t>
+        </is>
+      </c>
+      <c r="K30" t="n">
+        <v>407</v>
+      </c>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr"/>
+      <c r="O30" s="6" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
+      <c r="Q30" t="inlineStr"/>
+      <c r="R30" t="inlineStr"/>
+      <c r="S30" s="6" t="inlineStr"/>
+      <c r="T30" t="inlineStr"/>
+      <c r="U30" s="6" t="inlineStr"/>
+      <c r="V30" t="inlineStr"/>
+      <c r="W30" t="inlineStr"/>
+      <c r="X30" t="inlineStr"/>
+      <c r="Y30" t="inlineStr"/>
+      <c r="Z30" t="inlineStr"/>
+      <c r="AA30" s="6" t="inlineStr"/>
+      <c r="AB30" t="inlineStr"/>
     </row>
     <row r="31" ht="30" customHeight="1">
-      <c r="O31" s="6" t="n"/>
-      <c r="S31" s="6" t="n"/>
-      <c r="U31" s="6" t="n"/>
-      <c r="AA31" s="6" t="n"/>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Cliente | Transportadora</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Pessoa Física</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>627.058.194-01</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>João Guilherme da Paz</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Isento</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr"/>
+      <c r="O31" s="6" t="inlineStr"/>
+      <c r="P31" t="inlineStr"/>
+      <c r="Q31" t="inlineStr"/>
+      <c r="R31" t="inlineStr"/>
+      <c r="S31" s="6" t="inlineStr"/>
+      <c r="T31" t="inlineStr"/>
+      <c r="U31" s="6" t="inlineStr"/>
+      <c r="V31" t="inlineStr"/>
+      <c r="W31" t="inlineStr"/>
+      <c r="X31" t="inlineStr"/>
+      <c r="Y31" t="inlineStr"/>
+      <c r="Z31" t="inlineStr"/>
+      <c r="AA31" s="6" t="inlineStr"/>
+      <c r="AB31" t="inlineStr"/>
     </row>
     <row r="32" ht="30" customHeight="1">
-      <c r="O32" s="6" t="n"/>
-      <c r="S32" s="6" t="n"/>
-      <c r="U32" s="6" t="n"/>
-      <c r="AA32" s="6" t="n"/>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Cliente</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Estrangeiro</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>87149632050</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Ana Laura Porto</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Não Contribuinte</t>
+        </is>
+      </c>
+      <c r="K32" t="n">
+        <v>7607</v>
+      </c>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
+      <c r="O32" s="6" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
+      <c r="Q32" t="inlineStr"/>
+      <c r="R32" t="inlineStr"/>
+      <c r="S32" s="6" t="inlineStr"/>
+      <c r="T32" t="inlineStr"/>
+      <c r="U32" s="6" t="inlineStr"/>
+      <c r="V32" t="inlineStr"/>
+      <c r="W32" t="inlineStr"/>
+      <c r="X32" t="inlineStr"/>
+      <c r="Y32" t="inlineStr"/>
+      <c r="Z32" t="inlineStr"/>
+      <c r="AA32" s="6" t="inlineStr"/>
+      <c r="AB32" t="inlineStr"/>
     </row>
     <row r="33" ht="30" customHeight="1">
-      <c r="O33" s="6" t="n"/>
-      <c r="S33" s="6" t="n"/>
-      <c r="U33" s="6" t="n"/>
-      <c r="AA33" s="6" t="n"/>
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Transportadora</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Pessoa Jurídica</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>30.915.284/0001-07</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Sofia das Neves</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Contribuinte</t>
+        </is>
+      </c>
+      <c r="K33" t="n">
+        <v>9452</v>
+      </c>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
+      <c r="N33" t="inlineStr"/>
+      <c r="O33" s="6" t="inlineStr"/>
+      <c r="P33" t="inlineStr"/>
+      <c r="Q33" t="inlineStr"/>
+      <c r="R33" t="inlineStr"/>
+      <c r="S33" s="6" t="inlineStr"/>
+      <c r="T33" t="inlineStr"/>
+      <c r="U33" s="6" t="inlineStr"/>
+      <c r="V33" t="inlineStr"/>
+      <c r="W33" t="inlineStr"/>
+      <c r="X33" t="inlineStr"/>
+      <c r="Y33" t="inlineStr"/>
+      <c r="Z33" t="inlineStr"/>
+      <c r="AA33" s="6" t="inlineStr"/>
+      <c r="AB33" t="inlineStr"/>
     </row>
     <row r="34" ht="30" customHeight="1">
-      <c r="O34" s="6" t="n"/>
-      <c r="S34" s="6" t="n"/>
-      <c r="U34" s="6" t="n"/>
-      <c r="AA34" s="6" t="n"/>
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Cliente | Transportadora</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Pessoa Jurídica</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>69.830.452/0001-05</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Maria Luiza Nogueira</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Contribuinte</t>
+        </is>
+      </c>
+      <c r="K34" t="n">
+        <v>2284</v>
+      </c>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
+      <c r="N34" t="inlineStr"/>
+      <c r="O34" s="6" t="inlineStr"/>
+      <c r="P34" t="inlineStr"/>
+      <c r="Q34" t="inlineStr"/>
+      <c r="R34" t="inlineStr"/>
+      <c r="S34" s="6" t="inlineStr"/>
+      <c r="T34" t="inlineStr"/>
+      <c r="U34" s="6" t="inlineStr"/>
+      <c r="V34" t="inlineStr"/>
+      <c r="W34" t="inlineStr"/>
+      <c r="X34" t="inlineStr"/>
+      <c r="Y34" t="inlineStr"/>
+      <c r="Z34" t="inlineStr"/>
+      <c r="AA34" s="6" t="inlineStr"/>
+      <c r="AB34" t="inlineStr"/>
     </row>
     <row r="35" ht="30" customHeight="1">
-      <c r="O35" s="6" t="n"/>
-      <c r="S35" s="6" t="n"/>
-      <c r="U35" s="6" t="n"/>
-      <c r="AA35" s="6" t="n"/>
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Cliente | Transportadora</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Pessoa Jurídica</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>20.586.437/0001-66</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Alexandre Cavalcanti</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Não Contribuinte</t>
+        </is>
+      </c>
+      <c r="K35" t="n">
+        <v>5800</v>
+      </c>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
+      <c r="N35" t="inlineStr"/>
+      <c r="O35" s="6" t="inlineStr"/>
+      <c r="P35" t="inlineStr"/>
+      <c r="Q35" t="inlineStr"/>
+      <c r="R35" t="inlineStr"/>
+      <c r="S35" s="6" t="inlineStr"/>
+      <c r="T35" t="inlineStr"/>
+      <c r="U35" s="6" t="inlineStr"/>
+      <c r="V35" t="inlineStr"/>
+      <c r="W35" t="inlineStr"/>
+      <c r="X35" t="inlineStr"/>
+      <c r="Y35" t="inlineStr"/>
+      <c r="Z35" t="inlineStr"/>
+      <c r="AA35" s="6" t="inlineStr"/>
+      <c r="AB35" t="inlineStr"/>
     </row>
     <row r="36" ht="30" customHeight="1">
       <c r="O36" s="6" t="n"/>

</xml_diff>

<commit_message>
Ajustes repositoriesMongo implementado checkEmail
</commit_message>
<xml_diff>
--- a/excel/planilhasGerada/importar-parceiros.xlsx
+++ b/excel/planilhasGerada/importar-parceiros.xlsx
@@ -900,22 +900,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Cliente | Fornecedor</t>
+          <t>Cliente | Transportadora</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Pessoa Física</t>
+          <t>Estrangeiro</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>936.018.254-06</t>
+          <t>31768490287</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Sra. Daniela Gonçalves</t>
+          <t>Erick Santos</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
@@ -928,7 +928,7 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>1308</v>
+        <v>3947</v>
       </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
@@ -956,7 +956,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Fornecedor</t>
+          <t>Transportadora</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -966,12 +966,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>80153726903</t>
+          <t>02574891341</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Lívia Barros</t>
+          <t>Theo Pereira</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -980,10 +980,12 @@
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Isento</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr"/>
+          <t>Contribuinte</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>5578</v>
+      </c>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
@@ -1010,7 +1012,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Fornecedor</t>
+          <t>Cliente | Transportadora</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1020,12 +1022,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>75.061.498/0001-00</t>
+          <t>29.758.106/0001-30</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Caroline da Luz</t>
+          <t>Pietra Moreira</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
@@ -1034,12 +1036,10 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Contribuinte</t>
-        </is>
-      </c>
-      <c r="K5" t="n">
-        <v>7745</v>
-      </c>
+          <t>Isento</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
@@ -1059,502 +1059,58 @@
       <c r="AB5" t="inlineStr"/>
     </row>
     <row r="6" ht="30" customHeight="1">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Fornecedor</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Estrangeiro</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>38679205400</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Dra. Eloah da Cunha</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>Isento</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" s="6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" s="6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" s="6" t="inlineStr"/>
-      <c r="V6" t="inlineStr"/>
-      <c r="W6" t="inlineStr"/>
-      <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="inlineStr"/>
-      <c r="Z6" t="inlineStr"/>
-      <c r="AA6" s="6" t="inlineStr"/>
-      <c r="AB6" t="inlineStr"/>
+      <c r="O6" s="6" t="n"/>
+      <c r="S6" s="6" t="n"/>
+      <c r="U6" s="6" t="n"/>
+      <c r="AA6" s="6" t="n"/>
     </row>
     <row r="7" ht="30" customHeight="1">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Cliente | Fornecedor</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Estrangeiro</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>63790215406</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Marcos Vinicius Costela</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Isento</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" s="6" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" s="6" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" s="6" t="inlineStr"/>
-      <c r="V7" t="inlineStr"/>
-      <c r="W7" t="inlineStr"/>
-      <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="inlineStr"/>
-      <c r="Z7" t="inlineStr"/>
-      <c r="AA7" s="6" t="inlineStr"/>
-      <c r="AB7" t="inlineStr"/>
+      <c r="O7" s="6" t="n"/>
+      <c r="S7" s="6" t="n"/>
+      <c r="U7" s="6" t="n"/>
+      <c r="AA7" s="6" t="n"/>
     </row>
     <row r="8" ht="30" customHeight="1">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Fornecedor | Transportadora</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Estrangeiro</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>92308546115</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Dr. Nathan Cavalcanti</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Contribuinte</t>
-        </is>
-      </c>
-      <c r="K8" t="n">
-        <v>7270</v>
-      </c>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" s="6" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" s="6" t="inlineStr"/>
-      <c r="T8" t="inlineStr"/>
-      <c r="U8" s="6" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="inlineStr"/>
-      <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr"/>
-      <c r="Z8" t="inlineStr"/>
-      <c r="AA8" s="6" t="inlineStr"/>
-      <c r="AB8" t="inlineStr"/>
+      <c r="O8" s="6" t="n"/>
+      <c r="S8" s="6" t="n"/>
+      <c r="U8" s="6" t="n"/>
+      <c r="AA8" s="6" t="n"/>
     </row>
     <row r="9" ht="30" customHeight="1">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Fornecedor</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Estrangeiro</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>48073169584</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Maria Eduarda Correia</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>Não Contribuinte</t>
-        </is>
-      </c>
-      <c r="K9" t="n">
-        <v>5328</v>
-      </c>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" s="6" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" s="6" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
-      <c r="U9" s="6" t="inlineStr"/>
-      <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr"/>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
-      <c r="Z9" t="inlineStr"/>
-      <c r="AA9" s="6" t="inlineStr"/>
-      <c r="AB9" t="inlineStr"/>
+      <c r="O9" s="6" t="n"/>
+      <c r="S9" s="6" t="n"/>
+      <c r="U9" s="6" t="n"/>
+      <c r="AA9" s="6" t="n"/>
     </row>
     <row r="10" ht="30" customHeight="1">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Cliente | Transportadora</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Estrangeiro</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>98240531660</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Camila Lopes</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Isento</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" s="6" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" s="6" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" s="6" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr"/>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="inlineStr"/>
-      <c r="AA10" s="6" t="inlineStr"/>
-      <c r="AB10" t="inlineStr"/>
+      <c r="O10" s="6" t="n"/>
+      <c r="S10" s="6" t="n"/>
+      <c r="U10" s="6" t="n"/>
+      <c r="AA10" s="6" t="n"/>
     </row>
     <row r="11" ht="30" customHeight="1">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Cliente</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Pessoa Física</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>782.541.630-90</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Antônio da Cruz</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Contribuinte</t>
-        </is>
-      </c>
-      <c r="K11" t="n">
-        <v>7393</v>
-      </c>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" s="6" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" s="6" t="inlineStr"/>
-      <c r="T11" t="inlineStr"/>
-      <c r="U11" s="6" t="inlineStr"/>
-      <c r="V11" t="inlineStr"/>
-      <c r="W11" t="inlineStr"/>
-      <c r="X11" t="inlineStr"/>
-      <c r="Y11" t="inlineStr"/>
-      <c r="Z11" t="inlineStr"/>
-      <c r="AA11" s="6" t="inlineStr"/>
-      <c r="AB11" t="inlineStr"/>
+      <c r="O11" s="6" t="n"/>
+      <c r="S11" s="6" t="n"/>
+      <c r="U11" s="6" t="n"/>
+      <c r="AA11" s="6" t="n"/>
     </row>
     <row r="12" ht="30" customHeight="1">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Cliente | Transportadora</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Pessoa Jurídica</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>69.842.173/0001-53</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Heloísa da Rosa</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Contribuinte</t>
-        </is>
-      </c>
-      <c r="K12" t="n">
-        <v>9140</v>
-      </c>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" s="6" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" s="6" t="inlineStr"/>
-      <c r="T12" t="inlineStr"/>
-      <c r="U12" s="6" t="inlineStr"/>
-      <c r="V12" t="inlineStr"/>
-      <c r="W12" t="inlineStr"/>
-      <c r="X12" t="inlineStr"/>
-      <c r="Y12" t="inlineStr"/>
-      <c r="Z12" t="inlineStr"/>
-      <c r="AA12" s="6" t="inlineStr"/>
-      <c r="AB12" t="inlineStr"/>
+      <c r="O12" s="6" t="n"/>
+      <c r="S12" s="6" t="n"/>
+      <c r="U12" s="6" t="n"/>
+      <c r="AA12" s="6" t="n"/>
     </row>
     <row r="13" ht="30" customHeight="1">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Cliente</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Pessoa Jurídica</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>37.682.054/0001-94</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Alícia Caldeira</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>Contribuinte</t>
-        </is>
-      </c>
-      <c r="K13" t="n">
-        <v>6943</v>
-      </c>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" s="6" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" s="6" t="inlineStr"/>
-      <c r="T13" t="inlineStr"/>
-      <c r="U13" s="6" t="inlineStr"/>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr"/>
-      <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="inlineStr"/>
-      <c r="Z13" t="inlineStr"/>
-      <c r="AA13" s="6" t="inlineStr"/>
-      <c r="AB13" t="inlineStr"/>
+      <c r="O13" s="6" t="n"/>
+      <c r="S13" s="6" t="n"/>
+      <c r="U13" s="6" t="n"/>
+      <c r="AA13" s="6" t="n"/>
     </row>
     <row r="14" ht="30" customHeight="1">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Cliente | Fornecedor</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Pessoa Jurídica</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>93.546.107/0001-10</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Dr. Enzo Gabriel Santos</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>Não Contribuinte</t>
-        </is>
-      </c>
-      <c r="K14" t="n">
-        <v>1513</v>
-      </c>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" s="6" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" s="6" t="inlineStr"/>
-      <c r="T14" t="inlineStr"/>
-      <c r="U14" s="6" t="inlineStr"/>
-      <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr"/>
-      <c r="X14" t="inlineStr"/>
-      <c r="Y14" t="inlineStr"/>
-      <c r="Z14" t="inlineStr"/>
-      <c r="AA14" s="6" t="inlineStr"/>
-      <c r="AB14" t="inlineStr"/>
+      <c r="O14" s="6" t="n"/>
+      <c r="S14" s="6" t="n"/>
+      <c r="U14" s="6" t="n"/>
+      <c r="AA14" s="6" t="n"/>
     </row>
     <row r="15" ht="30" customHeight="1">
       <c r="O15" s="6" t="n"/>

</xml_diff>

<commit_message>
Ajustes ConnectionMongo Dev and Homolog
</commit_message>
<xml_diff>
--- a/excel/planilhasGerada/importar-parceiros.xlsx
+++ b/excel/planilhasGerada/importar-parceiros.xlsx
@@ -905,17 +905,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Estrangeiro</t>
+          <t>Pessoa Física</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>54901628720</t>
+          <t>169.703.482-96</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Alice Gonçalves</t>
+          <t>Elisa Barbosa</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
@@ -924,11 +924,11 @@
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Não Contribuinte</t>
+          <t>Contribuinte</t>
         </is>
       </c>
       <c r="K3" t="n">
-        <v>4603</v>
+        <v>7973</v>
       </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
@@ -956,22 +956,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cliente | Fornecedor</t>
+          <t>Transportadora</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Estrangeiro</t>
+          <t>Pessoa Física</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>35924106870</t>
+          <t>362.740.195-61</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Gabriel da Cruz</t>
+          <t>Isabel Aragão</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -980,10 +980,12 @@
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Isento</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr"/>
+          <t>Não Contribuinte</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>7426</v>
+      </c>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
@@ -1010,22 +1012,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Fornecedor</t>
+          <t>Cliente | Fornecedor | Transportadora</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Pessoa Física</t>
+          <t>Pessoa Jurídica</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>386.957.240-00</t>
+          <t>73.928.645/0001-62</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Lara da Costa</t>
+          <t>Pedro Henrique Azevedo</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
@@ -1034,12 +1036,10 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Contribuinte</t>
-        </is>
-      </c>
-      <c r="K5" t="n">
-        <v>3188</v>
-      </c>
+          <t>Isento</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
@@ -1066,22 +1066,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Cliente | Fornecedor</t>
+          <t>Cliente</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Estrangeiro</t>
+          <t>Pessoa Jurídica</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>23149657873</t>
+          <t>29.378.604/0001-58</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Cauã Cardoso</t>
+          <t>Lara Souza</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
@@ -1094,7 +1094,7 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>44</v>
+        <v>927</v>
       </c>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
@@ -1132,12 +1132,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>13.924.768/0001-01</t>
+          <t>13.407.625/0001-14</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Luiz Felipe da Rosa</t>
+          <t>Srta. Letícia Cardoso</t>
         </is>
       </c>
       <c r="F7" t="inlineStr"/>
@@ -1146,11 +1146,11 @@
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Não Contribuinte</t>
+          <t>Contribuinte</t>
         </is>
       </c>
       <c r="K7" t="n">
-        <v>4271</v>
+        <v>3365</v>
       </c>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
@@ -1178,22 +1178,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Cliente | Fornecedor | Transportadora</t>
+          <t>Cliente | Fornecedor</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Pessoa Física</t>
+          <t>Pessoa Jurídica</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>269.301.584-70</t>
+          <t>08.571.926/0001-49</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Gustavo Campos</t>
+          <t>Sr. Breno Silveira</t>
         </is>
       </c>
       <c r="F8" t="inlineStr"/>
@@ -1202,10 +1202,12 @@
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Isento</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr"/>
+          <t>Não Contribuinte</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>3236</v>
+      </c>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
@@ -1232,22 +1234,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Cliente | Fornecedor | Transportadora</t>
+          <t>Fornecedor | Transportadora</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Estrangeiro</t>
+          <t>Pessoa Física</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>28340619551</t>
+          <t>054.796.213-43</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Sr. Alexandre Melo</t>
+          <t>Júlia Moreira</t>
         </is>
       </c>
       <c r="F9" t="inlineStr"/>
@@ -1260,7 +1262,7 @@
         </is>
       </c>
       <c r="K9" t="n">
-        <v>9132</v>
+        <v>6677</v>
       </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
@@ -1288,7 +1290,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Fornecedor | Transportadora</t>
+          <t>Cliente</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1298,12 +1300,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>50163289786</t>
+          <t>89165203470</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Maria Luiza Sales</t>
+          <t>Emilly Jesus</t>
         </is>
       </c>
       <c r="F10" t="inlineStr"/>
@@ -1312,12 +1314,10 @@
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Não Contribuinte</t>
-        </is>
-      </c>
-      <c r="K10" t="n">
-        <v>1349</v>
-      </c>
+          <t>Isento</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
@@ -1344,22 +1344,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Cliente | Fornecedor</t>
+          <t>Cliente</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Estrangeiro</t>
+          <t>Pessoa Jurídica</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>87961450300</t>
+          <t>63.548.791/0001-09</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Evelyn da Luz</t>
+          <t>Dr. Samuel Gomes</t>
         </is>
       </c>
       <c r="F11" t="inlineStr"/>
@@ -1368,10 +1368,12 @@
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Isento</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr"/>
+          <t>Contribuinte</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>8651</v>
+      </c>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
@@ -1398,22 +1400,22 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Fornecedor</t>
+          <t>Cliente | Fornecedor</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Pessoa Física</t>
+          <t>Estrangeiro</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>346.158.079-10</t>
+          <t>51382649070</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Beatriz Fogaça</t>
+          <t>Matheus Pereira</t>
         </is>
       </c>
       <c r="F12" t="inlineStr"/>
@@ -1422,10 +1424,12 @@
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Isento</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr"/>
+          <t>Contribuinte</t>
+        </is>
+      </c>
+      <c r="K12" t="n">
+        <v>6740</v>
+      </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
@@ -1452,22 +1456,22 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Transportadora</t>
+          <t>Cliente | Fornecedor | Transportadora</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Pessoa Jurídica</t>
+          <t>Estrangeiro</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>96.723.851/0001-31</t>
+          <t>47560829392</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Anthony Nogueira</t>
+          <t>Laís Correia</t>
         </is>
       </c>
       <c r="F13" t="inlineStr"/>
@@ -1476,11 +1480,11 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Contribuinte</t>
+          <t>Não Contribuinte</t>
         </is>
       </c>
       <c r="K13" t="n">
-        <v>5224</v>
+        <v>9738</v>
       </c>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
@@ -1508,22 +1512,22 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Fornecedor | Transportadora</t>
+          <t>Cliente | Fornecedor | Transportadora</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Estrangeiro</t>
+          <t>Pessoa Jurídica</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>09572816411</t>
+          <t>05.231.469/0001-55</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Murilo Peixoto</t>
+          <t>Isadora Santos</t>
         </is>
       </c>
       <c r="F14" t="inlineStr"/>
@@ -1532,11 +1536,11 @@
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Contribuinte</t>
+          <t>Não Contribuinte</t>
         </is>
       </c>
       <c r="K14" t="n">
-        <v>1260</v>
+        <v>7630</v>
       </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
@@ -1564,7 +1568,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Cliente | Fornecedor</t>
+          <t>Fornecedor</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1574,12 +1578,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>74.825.639/0001-42</t>
+          <t>81.236.590/0001-58</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Gabrielly Teixeira</t>
+          <t>Emilly Almeida</t>
         </is>
       </c>
       <c r="F15" t="inlineStr"/>
@@ -1588,12 +1592,10 @@
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Contribuinte</t>
-        </is>
-      </c>
-      <c r="K15" t="n">
-        <v>4900</v>
-      </c>
+          <t>Isento</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
@@ -1620,7 +1622,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Fornecedor | Transportadora</t>
+          <t>Cliente | Fornecedor</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1630,12 +1632,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>54027916867</t>
+          <t>17280453988</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Dra. Sofia Viana</t>
+          <t>Sabrina Duarte</t>
         </is>
       </c>
       <c r="F16" t="inlineStr"/>
@@ -1648,7 +1650,7 @@
         </is>
       </c>
       <c r="K16" t="n">
-        <v>5642</v>
+        <v>7694</v>
       </c>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
@@ -1676,22 +1678,22 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Cliente | Fornecedor | Transportadora</t>
+          <t>Transportadora</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Estrangeiro</t>
+          <t>Pessoa Jurídica</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>60159834775</t>
+          <t>84.135.279/0001-00</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Ryan da Cunha</t>
+          <t>Stella Pereira</t>
         </is>
       </c>
       <c r="F17" t="inlineStr"/>
@@ -1730,22 +1732,22 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Fornecedor | Transportadora</t>
+          <t>Transportadora</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Estrangeiro</t>
+          <t>Pessoa Física</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>50127934634</t>
+          <t>023.691.847-87</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Elisa Azevedo</t>
+          <t>Pietra Fogaça</t>
         </is>
       </c>
       <c r="F18" t="inlineStr"/>
@@ -1754,11 +1756,11 @@
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Contribuinte</t>
+          <t>Não Contribuinte</t>
         </is>
       </c>
       <c r="K18" t="n">
-        <v>7602</v>
+        <v>6188</v>
       </c>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr"/>
@@ -1791,17 +1793,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Estrangeiro</t>
+          <t>Pessoa Jurídica</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>14863970501</t>
+          <t>58.629.103/0001-03</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Daniela Monteiro</t>
+          <t>Bárbara Pinto</t>
         </is>
       </c>
       <c r="F19" t="inlineStr"/>
@@ -1810,11 +1812,11 @@
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Não Contribuinte</t>
+          <t>Contribuinte</t>
         </is>
       </c>
       <c r="K19" t="n">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
@@ -1842,22 +1844,22 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Cliente | Fornecedor</t>
+          <t>Fornecedor</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Pessoa Jurídica</t>
+          <t>Pessoa Física</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>96.413.258/0001-99</t>
+          <t>376.945.281-09</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Marina da Rocha</t>
+          <t>Giovanna Aragão</t>
         </is>
       </c>
       <c r="F20" t="inlineStr"/>
@@ -1866,12 +1868,10 @@
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Não Contribuinte</t>
-        </is>
-      </c>
-      <c r="K20" t="n">
-        <v>1980</v>
-      </c>
+          <t>Isento</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
@@ -1898,22 +1898,22 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Cliente | Fornecedor</t>
+          <t>Cliente | Transportadora</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Pessoa Jurídica</t>
+          <t>Pessoa Física</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>08.715.243/0001-18</t>
+          <t>837.261.405-90</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Maria Sophia Souza</t>
+          <t>Isabelly da Luz</t>
         </is>
       </c>
       <c r="F21" t="inlineStr"/>
@@ -1922,10 +1922,12 @@
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Isento</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr"/>
+          <t>Contribuinte</t>
+        </is>
+      </c>
+      <c r="K21" t="n">
+        <v>3181</v>
+      </c>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
@@ -1952,22 +1954,22 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Cliente | Transportadora</t>
+          <t>Cliente | Fornecedor</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Pessoa Física</t>
+          <t>Estrangeiro</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>054.296.831-24</t>
+          <t>85193672400</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Thiago Costa</t>
+          <t>Clarice Jesus</t>
         </is>
       </c>
       <c r="F22" t="inlineStr"/>
@@ -2006,22 +2008,22 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Fornecedor | Transportadora</t>
+          <t>Cliente | Fornecedor</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Pessoa Jurídica</t>
+          <t>Estrangeiro</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>03.957.142/0001-30</t>
+          <t>50381792404</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Gabriel da Mota</t>
+          <t>Sra. Maria Luiza Campos</t>
         </is>
       </c>
       <c r="F23" t="inlineStr"/>
@@ -2030,12 +2032,10 @@
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Contribuinte</t>
-        </is>
-      </c>
-      <c r="K23" t="n">
-        <v>2177</v>
-      </c>
+          <t>Isento</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
@@ -2062,7 +2062,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Cliente | Fornecedor | Transportadora</t>
+          <t>Fornecedor | Transportadora</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -2072,12 +2072,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>56.902.134/0001-52</t>
+          <t>34.276.510/0001-08</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Maria Vitória Monteiro</t>
+          <t>Carolina da Rocha</t>
         </is>
       </c>
       <c r="F24" t="inlineStr"/>
@@ -2086,10 +2086,12 @@
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Isento</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr"/>
+          <t>Não Contribuinte</t>
+        </is>
+      </c>
+      <c r="K24" t="n">
+        <v>1073</v>
+      </c>
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
@@ -2109,58 +2111,10 @@
       <c r="AB24" t="inlineStr"/>
     </row>
     <row r="25" ht="30" customHeight="1">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Transportadora</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Pessoa Jurídica</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>74.951.382/0001-75</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Gabrielly Azevedo</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>Isento</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="inlineStr"/>
-      <c r="O25" s="6" t="inlineStr"/>
-      <c r="P25" t="inlineStr"/>
-      <c r="Q25" t="inlineStr"/>
-      <c r="R25" t="inlineStr"/>
-      <c r="S25" s="6" t="inlineStr"/>
-      <c r="T25" t="inlineStr"/>
-      <c r="U25" s="6" t="inlineStr"/>
-      <c r="V25" t="inlineStr"/>
-      <c r="W25" t="inlineStr"/>
-      <c r="X25" t="inlineStr"/>
-      <c r="Y25" t="inlineStr"/>
-      <c r="Z25" t="inlineStr"/>
-      <c r="AA25" s="6" t="inlineStr"/>
-      <c r="AB25" t="inlineStr"/>
+      <c r="O25" s="6" t="n"/>
+      <c r="S25" s="6" t="n"/>
+      <c r="U25" s="6" t="n"/>
+      <c r="AA25" s="6" t="n"/>
     </row>
     <row r="26" ht="30" customHeight="1">
       <c r="O26" s="6" t="n"/>

</xml_diff>